<commit_message>
crated test fildefault print location launch filee, solved path to excelpy file, solved
</commit_message>
<xml_diff>
--- a/Final_Projects/InventoryProject/inventory.xlsx
+++ b/Final_Projects/InventoryProject/inventory.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>Product No</t>
   </si>
@@ -39,9 +39,6 @@
   <si>
     <t>CCC Company</t>
   </si>
-  <si>
-    <t/>
-  </si>
 </sst>
 </file>
 
@@ -58,7 +55,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -90,7 +87,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -101,6 +98,9 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -116,17 +116,8 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -436,14 +427,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="10" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="13.719285714285713" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="10" width="12.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -460,269 +451,267 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="16.5">
-      <c r="A2" s="4">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="5">
         <v>20</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="6">
         <v>200.4</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4">
-        <f>B2*C2</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="16.5">
-      <c r="A3" s="4">
+      <c r="E2" s="5">
+        <v>4008</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="5">
         <v>23</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="5">
         <v>33</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="4">
-        <f>B3*C3</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="16.5">
-      <c r="A4" s="4">
+      <c r="E3" s="5">
+        <v>759</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="5">
         <v>30000</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="6">
         <v>234.99</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="4">
-        <f>B4*C4</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="16.5">
-      <c r="A5" s="4">
+      <c r="E4" s="5">
+        <v>7049700</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="5">
         <v>43</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="6">
         <v>21.89</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="5">
-        <f>B5*C5</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="16.5">
-      <c r="A6" s="4">
+      <c r="E5" s="6">
+        <v>941.27</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="5">
         <v>523</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="6">
         <v>55.99</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="5">
-        <f>B6*C6</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="16.5">
-      <c r="A7" s="4">
+      <c r="E6" s="6">
+        <v>29282.77</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="5">
         <v>54</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="5">
         <v>1150</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="4">
-        <f>B7*C7</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="16.5">
-      <c r="A8" s="4">
+      <c r="E7" s="5">
+        <v>62100</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="5">
         <v>352</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="6">
         <v>122.55</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="5">
-        <f>B8*C8</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="16.5">
-      <c r="A9" s="4">
+      <c r="E8" s="6">
+        <v>43137.6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="5">
         <v>2352</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="5">
         <v>111</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="4">
-        <f>B9*C9</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="16.5">
-      <c r="A10" s="4">
+      <c r="E9" s="5">
+        <v>261.072</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="5">
         <v>666</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="6">
         <v>345.99</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="5">
-        <f>B10*C10</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="16.5">
-      <c r="A11" s="6">
+      <c r="E10" s="6">
+        <v>230429.3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>55</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>605.32</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="5">
-        <f>B11*C11</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="16.5">
-      <c r="A12" s="6">
+      <c r="E11" s="6">
+        <v>33292.6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>6</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>66.11</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="5">
-        <f>B12*C12</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="16.5">
-      <c r="A13" s="6">
+      <c r="E12" s="6">
+        <v>396.66</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>47</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>112.12</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="5">
-        <f>B13*C13</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="16.5">
-      <c r="A14" s="6">
+      <c r="E13" s="6">
+        <v>5269.64</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>69</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>45.32</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="5">
-        <f>B14*C14</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="16.5">
-      <c r="A15" s="4">
+      <c r="E14" s="6">
+        <v>3127</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="5">
         <v>235</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="6">
         <v>6466.95</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="5">
-        <f>B15*C15</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="16.5">
-      <c r="A16" s="4">
+      <c r="E15" s="6">
+        <v>1519733.25</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="5">
         <v>77</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="6">
         <v>13.99</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="5">
-        <f>B16*C16</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="16.5">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="5">
+      <c r="E16" s="6">
+        <v>1077.23</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="6">
         <f>sum(e2:e16)</f>
       </c>
     </row>

</xml_diff>